<commit_message>
EPBDS-1587 add convertors for BigInteger, BigDecimal. tests
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/datatype/DatatypeDefaultValues.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/datatype/DatatypeDefaultValues.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Datatype TestType</t>
   </si>
@@ -121,6 +121,24 @@
   </si>
   <si>
     <t>fgfs</t>
+  </si>
+  <si>
+    <t>Datatype TestBigTypes</t>
+  </si>
+  <si>
+    <t>BigInteger</t>
+  </si>
+  <si>
+    <t>bigIntVal</t>
+  </si>
+  <si>
+    <t>bigDecVal</t>
+  </si>
+  <si>
+    <t>BigDecimal</t>
+  </si>
+  <si>
+    <t>bigIntVal2</t>
   </si>
 </sst>
 </file>
@@ -171,10 +189,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -475,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:L19"/>
+  <dimension ref="B3:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD27"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -492,16 +516,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:12">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="G3" s="4" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="G3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="2:12">
       <c r="B4" s="1" t="s">
@@ -604,16 +628,16 @@
       </c>
     </row>
     <row r="15" spans="2:12">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="J15" s="4" t="s">
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="J15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
     </row>
     <row r="16" spans="2:12">
       <c r="B16" s="3" t="s">
@@ -637,7 +661,7 @@
       <c r="B17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="1">
@@ -669,12 +693,51 @@
         <v>29</v>
       </c>
     </row>
+    <row r="22" spans="2:12">
+      <c r="B22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="2:12">
+      <c r="B23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2000000000</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12">
+      <c r="B24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1115.3699999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12">
+      <c r="B25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="J15:L15"/>
+    <mergeCell ref="B22:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>